<commit_message>
First stage of adapting to project's problem
</commit_message>
<xml_diff>
--- a/scheduling.xlsx
+++ b/scheduling.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afdav\Documents\Repos\schedule-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B7CF5-863C-48CB-8444-FD80D1D4FD2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE29C7BD-090F-4444-8630-3CCAC1F59380}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="510" windowWidth="19425" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17895" yWindow="960" windowWidth="19425" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Available" sheetId="2" r:id="rId1"/>
-    <sheet name="Required" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Instructors" sheetId="2" r:id="rId1"/>
+    <sheet name="Students" sheetId="4" r:id="rId2"/>
+    <sheet name="Required" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Staff Requirement</t>
     <phoneticPr fontId="1"/>
@@ -101,6 +102,63 @@
   </si>
   <si>
     <t>CAS-6</t>
+  </si>
+  <si>
+    <t>TR-4</t>
+  </si>
+  <si>
+    <t>ISR-3</t>
+  </si>
+  <si>
+    <t>SCAR-2</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>ValueForCompleting</t>
+  </si>
+  <si>
+    <t>TR-1</t>
+  </si>
+  <si>
+    <t>TR-2</t>
+  </si>
+  <si>
+    <t>TR-3</t>
+  </si>
+  <si>
+    <t>TR-5</t>
+  </si>
+  <si>
+    <t>ISR-1</t>
+  </si>
+  <si>
+    <t>ISR-2</t>
+  </si>
+  <si>
+    <t>ISR-4</t>
+  </si>
+  <si>
+    <t>ISR-5</t>
+  </si>
+  <si>
+    <t>SCAR-1</t>
+  </si>
+  <si>
+    <t>CAS-1</t>
+  </si>
+  <si>
+    <t>CAS-2</t>
+  </si>
+  <si>
+    <t>CAS-5</t>
+  </si>
+  <si>
+    <t>MinHours</t>
+  </si>
+  <si>
+    <t>MaxHours</t>
   </si>
 </sst>
 </file>
@@ -436,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,11 +503,11 @@
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -465,14 +523,8 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -480,20 +532,14 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -501,20 +547,14 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>50</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -528,50 +568,38 @@
         <v>30</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>30</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>40</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -586,7 +614,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -594,32 +622,32 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>45</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:5">
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:5">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:5">
       <c r="E11" s="1"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:5">
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:5">
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:5">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:5">
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="5:5">
@@ -645,6 +673,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4457E96C-9948-4907-888F-0CA9A2890FA6}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -703,14 +819,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create optimization for staff/studs
</commit_message>
<xml_diff>
--- a/scheduling.xlsx
+++ b/scheduling.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afdav\Documents\Repos\schedule-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE29C7BD-090F-4444-8630-3CCAC1F59380}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAF2558-C6D2-4650-83E5-FADB65545D21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="960" windowWidth="19425" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17895" yWindow="960" windowWidth="19425" windowHeight="15195" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructors" sheetId="2" r:id="rId1"/>
     <sheet name="Students" sheetId="4" r:id="rId2"/>
     <sheet name="Required" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Reward" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,17 +27,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1A55F813-2424-4425-8A47-2C3EA6ABE1ED}</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1A55F813-2424-4425-8A47-2C3EA6ABE1ED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is almost always going to be 1 but sometimes you have super sorties or other such events that require more</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
-    <t>Staff Requirement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Time (24H)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>EmployeeName</t>
   </si>
   <si>
@@ -159,13 +169,19 @@
   </si>
   <si>
     <t>MaxHours</t>
+  </si>
+  <si>
+    <t>RideNum</t>
+  </si>
+  <si>
+    <t>CrewRequirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +196,12 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,6 +251,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Campbell,David" id="{B3D615DB-081C-48E9-83ED-FAB25C704820}" userId="Campbell,David" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,11 +520,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A2" dT="2019-12-05T07:15:49.64" personId="{B3D615DB-081C-48E9-83ED-FAB25C704820}" id="{1A55F813-2424-4425-8A47-2C3EA6ABE1ED}">
+    <text>This is almost always going to be 1 but sometimes you have super sorties or other such events that require more</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -509,24 +545,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -541,7 +577,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -556,7 +592,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -571,7 +607,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -586,7 +622,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -601,7 +637,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -616,7 +652,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -687,21 +723,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -710,12 +746,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -724,12 +760,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -738,12 +774,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -752,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -775,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -795,7 +831,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -816,6 +852,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -823,21 +860,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -845,7 +885,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -853,7 +893,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -861,7 +901,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -869,7 +909,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -877,7 +917,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -885,7 +925,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -893,7 +933,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -901,7 +941,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -909,7 +949,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -917,7 +957,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -925,7 +965,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -933,7 +973,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -941,7 +981,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -949,7 +989,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -957,7 +997,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -965,7 +1005,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -973,7 +1013,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>4</v>

</xml_diff>

<commit_message>
Only one student crew flying per time slot
</commit_message>
<xml_diff>
--- a/scheduling.xlsx
+++ b/scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afdav\Documents\Repos\schedule-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAF2558-C6D2-4650-83E5-FADB65545D21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7956B44B-41A1-4071-8CAE-7F4A17E77823}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="960" windowWidth="19425" windowHeight="15195" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="585" windowWidth="19425" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructors" sheetId="2" r:id="rId1"/>
@@ -532,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -568,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -610,10 +610,10 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -625,10 +625,10 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>40</v>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>45</v>
@@ -712,7 +712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4457E96C-9948-4907-888F-0CA9A2890FA6}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -860,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>